<commit_message>
updated docs to fit new structure
</commit_message>
<xml_diff>
--- a/docs/diagrams.xlsx
+++ b/docs/diagrams.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Preamble</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Transport Control</t>
   </si>
   <si>
-    <t>Mesh srv</t>
-  </si>
-  <si>
     <t>Trickle</t>
   </si>
   <si>
@@ -82,6 +79,18 @@
   </si>
   <si>
     <t>nRF51 Series IC</t>
+  </si>
+  <si>
+    <t>Mesh packet</t>
+  </si>
+  <si>
+    <t>Mesh Srv</t>
+  </si>
+  <si>
+    <t>Version handler</t>
+  </si>
+  <si>
+    <t>Event handler</t>
   </si>
 </sst>
 </file>
@@ -199,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -375,11 +384,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0"/>
+      </left>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
@@ -397,26 +459,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -469,31 +516,55 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -966,103 +1037,103 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="21" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="21"/>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="21"/>
-      <c r="AG3" s="21"/>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="21"/>
-      <c r="AK3" s="21"/>
-      <c r="AL3" s="21"/>
-      <c r="AM3" s="21"/>
-      <c r="AN3" s="21"/>
-      <c r="AO3" s="21"/>
-      <c r="AP3" s="21"/>
-      <c r="AQ3" s="21"/>
-      <c r="AR3" s="21"/>
-      <c r="AS3" s="21"/>
-      <c r="AT3" s="22" t="s">
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="16"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="16"/>
+      <c r="AR3" s="16"/>
+      <c r="AS3" s="16"/>
+      <c r="AT3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="AU3" s="23"/>
-      <c r="AV3" s="24"/>
+      <c r="AU3" s="18"/>
+      <c r="AV3" s="19"/>
     </row>
     <row r="9" spans="2:48" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="25" t="s">
+      <c r="K9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="26"/>
-      <c r="M9" s="27" t="s">
+      <c r="L9" s="21"/>
+      <c r="M9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
-      <c r="AE9" s="21"/>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="21"/>
-      <c r="AH9" s="21"/>
-      <c r="AI9" s="21"/>
-      <c r="AJ9" s="21"/>
-      <c r="AK9" s="21"/>
-      <c r="AL9" s="21"/>
-      <c r="AM9" s="21"/>
-      <c r="AN9" s="28"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="16"/>
+      <c r="AF9" s="16"/>
+      <c r="AG9" s="16"/>
+      <c r="AH9" s="16"/>
+      <c r="AI9" s="16"/>
+      <c r="AJ9" s="16"/>
+      <c r="AK9" s="16"/>
+      <c r="AL9" s="16"/>
+      <c r="AM9" s="16"/>
+      <c r="AN9" s="23"/>
     </row>
     <row r="10" spans="2:48" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="J10" s="5">
@@ -1180,118 +1251,137 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="385" zoomScaleNormal="385" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="3" max="8" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
-    <row r="2" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="31" t="s">
+    <row r="2" spans="1:11" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33"/>
+      <c r="B2" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="33"/>
+      <c r="B3" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="1:11" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="28"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+    </row>
+    <row r="7" spans="1:11" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35"/>
+      <c r="B7" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="6"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
     </row>
-    <row r="3" spans="1:7" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+    <row r="8" spans="1:11" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="35"/>
-    </row>
-    <row r="6" spans="1:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="6"/>
+    <row r="9" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="C4:E4"/>
+  <mergeCells count="10">
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>